<commit_message>
Chose numbers that made more sense
</commit_message>
<xml_diff>
--- a/RCL-B-CDH1 Data Budget.xlsx
+++ b/RCL-B-CDH1 Data Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="12600" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="0" windowWidth="12600" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="2" r:id="rId1"/>
@@ -12,17 +12,21 @@
   </sheets>
   <definedNames>
     <definedName name="f_save">Assumptions!$C$5</definedName>
+    <definedName name="fps">Assumptions!$C$5</definedName>
     <definedName name="IFPS">Assumptions!$C$2</definedName>
+    <definedName name="ISKS">Assumptions!$C$2</definedName>
     <definedName name="mem">Assumptions!$C$6</definedName>
     <definedName name="RFPS">Assumptions!$C$4</definedName>
+    <definedName name="RSKS">Assumptions!$C$4</definedName>
     <definedName name="TFPS">Assumptions!$C$3</definedName>
+    <definedName name="TS">Assumptions!$C$3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>Data size</t>
   </si>
@@ -69,30 +73,6 @@
     <t>Transition</t>
   </si>
   <si>
-    <t>ISK fps</t>
-  </si>
-  <si>
-    <t>Transition fps</t>
-  </si>
-  <si>
-    <t>RSK fps</t>
-  </si>
-  <si>
-    <t>frame to save</t>
-  </si>
-  <si>
-    <t>IFPS</t>
-  </si>
-  <si>
-    <t>TFPS</t>
-  </si>
-  <si>
-    <t>RFPS</t>
-  </si>
-  <si>
-    <t>f_save</t>
-  </si>
-  <si>
     <t>Memory size</t>
   </si>
   <si>
@@ -111,9 +91,6 @@
     <t>fps</t>
   </si>
   <si>
-    <t>th frame</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -121,6 +98,30 @@
   </si>
   <si>
     <t>(Hz)</t>
+  </si>
+  <si>
+    <t>FPS</t>
+  </si>
+  <si>
+    <t>RSK Sampling</t>
+  </si>
+  <si>
+    <t>Transition Sampling</t>
+  </si>
+  <si>
+    <t>ISK Sampling</t>
+  </si>
+  <si>
+    <t>ISKS</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>RSKS</t>
+  </si>
+  <si>
+    <t>frame #</t>
   </si>
 </sst>
 </file>
@@ -162,7 +163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -354,6 +355,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -361,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,7 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,12 +425,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -789,97 +822,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="22">
+        <v>60</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="27" t="s">
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="23">
+        <v>60</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="C4" s="23">
+        <v>60</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="23">
+        <v>30</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="23">
-        <v>8</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="25">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="24">
-        <v>4</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="24">
-        <v>2</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="24">
-        <v>20</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="26">
-        <v>8</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -888,6 +922,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -895,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,24 +961,24 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -953,50 +988,51 @@
         <f>9.83*10^6</f>
         <v>9830000</v>
       </c>
-      <c r="D4" s="22">
-        <f>IFPS*(1/f_save)</f>
-        <v>0.4</v>
-      </c>
-      <c r="E4" s="19">
+      <c r="D4" s="21">
+        <f>fps/ISKS</f>
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="18">
         <f>C4*(60*D4)</f>
-        <v>235920000</v>
+        <v>294900000</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="7">
-        <v>24</v>
+        <f>24*8</f>
+        <v>192</v>
       </c>
       <c r="D5" s="7">
-        <f>IFPS</f>
-        <v>8</v>
-      </c>
-      <c r="E5" s="18">
+        <f>fps</f>
+        <v>30</v>
+      </c>
+      <c r="E5" s="17">
         <f>C5*60*D5</f>
-        <v>11520</v>
+        <v>345600</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="14"/>
-      <c r="E6" s="20">
+      <c r="A6" s="12"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="13"/>
+      <c r="E6" s="19">
         <f>SUM(E4:E5)</f>
-        <v>235931520</v>
+        <v>295245600</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="13"/>
       <c r="E7" s="9">
         <f>180</f>
         <v>180</v>
@@ -1006,22 +1042,22 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="14"/>
-      <c r="E8" s="20">
+      <c r="A8" s="11"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="13"/>
+      <c r="E8" s="19">
         <f>E7*E6</f>
-        <v>42467673600</v>
+        <v>53144208000</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1042,24 +1078,24 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="D12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1069,65 +1105,66 @@
         <f>9.83*10^6</f>
         <v>9830000</v>
       </c>
-      <c r="D13" s="22">
-        <f>TFPS*(1/f_save)</f>
-        <v>0.2</v>
-      </c>
-      <c r="E13" s="19">
+      <c r="D13" s="21">
+        <f>fps/TS</f>
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="18">
         <f>C13*(60*D13)</f>
-        <v>117960000</v>
+        <v>294900000</v>
       </c>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="7">
-        <v>24</v>
+        <f>24*8</f>
+        <v>192</v>
       </c>
       <c r="D14" s="7">
-        <f>(TFPS)</f>
-        <v>4</v>
-      </c>
-      <c r="E14" s="18">
+        <f>fps</f>
+        <v>30</v>
+      </c>
+      <c r="E14" s="17">
         <f>C14*60*D14</f>
-        <v>5760</v>
+        <v>345600</v>
       </c>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="14"/>
-      <c r="E15" s="20">
+      <c r="A15" s="12"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="13"/>
+      <c r="E15" s="19">
         <f>SUM(E13:E14)</f>
-        <v>117965760</v>
+        <v>295245600</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="13"/>
       <c r="E16" s="9">
-        <f>90</f>
-        <v>90</v>
+        <f>90*2</f>
+        <v>180</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="14"/>
-      <c r="E17" s="20">
+      <c r="A17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="13"/>
+      <c r="E17" s="19">
         <f>E16*E15</f>
-        <v>10616918400</v>
+        <v>53144208000</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -1152,24 +1189,24 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="17" t="s">
+      <c r="D21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1179,50 +1216,51 @@
         <f>9.83*10^6</f>
         <v>9830000</v>
       </c>
-      <c r="D22" s="22">
-        <f>RFPS*(1/f_save)</f>
-        <v>0.1</v>
-      </c>
-      <c r="E22" s="19">
+      <c r="D22" s="21">
+        <f>fps/RSKS</f>
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="18">
         <f>C22*(60*D22)</f>
-        <v>58980000</v>
+        <v>294900000</v>
       </c>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="7">
-        <v>24</v>
+        <f>24*8</f>
+        <v>192</v>
       </c>
       <c r="D23" s="7">
-        <f>RFPS</f>
-        <v>2</v>
-      </c>
-      <c r="E23" s="18">
+        <f>fps</f>
+        <v>30</v>
+      </c>
+      <c r="E23" s="17">
         <f>C23*60*D23</f>
-        <v>2880</v>
+        <v>345600</v>
       </c>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="14"/>
-      <c r="E24" s="20">
+      <c r="A24" s="12"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="13"/>
+      <c r="E24" s="19">
         <f>SUM(E22:E23)</f>
-        <v>58982880</v>
+        <v>295245600</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="14"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="13"/>
       <c r="E25" s="9">
         <f>90</f>
         <v>90</v>
@@ -1232,42 +1270,42 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="14"/>
-      <c r="E26" s="20">
+      <c r="A26" s="11"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="13"/>
+      <c r="E26" s="19">
         <f>E25*E24</f>
-        <v>5308459200</v>
+        <v>26572104000</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="20">
+      <c r="E28" s="19">
         <f>SUM(E8,E15,E26)</f>
-        <v>47894098560</v>
+        <v>80011557600</v>
       </c>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E29" s="8">
         <f>mem-(mem*0.25)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="21">
+      <c r="E30" s="20">
         <f>0.125*E28*(10^-9)</f>
-        <v>5.9867623200000004</v>
+        <v>10.0014447</v>
       </c>
       <c r="F30" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1277,36 +1315,46 @@
     <mergeCell ref="A22:A23"/>
   </mergeCells>
   <conditionalFormatting sqref="E7 C4:E5">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16 D14:E14 C13:D13">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25 D23:E23 C22:D22">
     <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16 C14:E14 C13:D13">
+  <conditionalFormatting sqref="E13">
     <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25 C23:E23 C22:D22">
+  <conditionalFormatting sqref="E22">
     <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+  <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>$E$29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+      <formula>$E$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+  <conditionalFormatting sqref="C23">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>$E$29</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
-      <formula>$E$29</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed a mistake and made a chart to move 2 ppt
</commit_message>
<xml_diff>
--- a/RCL-B-CDH1 Data Budget.xlsx
+++ b/RCL-B-CDH1 Data Budget.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="12600" windowHeight="12390"/>
+    <workbookView xWindow="-15" yWindow="0" windowWidth="12600" windowHeight="12390" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="2" r:id="rId1"/>
     <sheet name="Data Budget" sheetId="1" r:id="rId2"/>
+    <sheet name="For Pie" sheetId="3" r:id="rId3"/>
+    <sheet name="Pretty Pie Chart" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="f_save">Assumptions!$C$5</definedName>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>Data size</t>
   </si>
@@ -122,6 +124,27 @@
   </si>
   <si>
     <t>frame #</t>
+  </si>
+  <si>
+    <t>Mission Segment</t>
+  </si>
+  <si>
+    <t>ISK</t>
+  </si>
+  <si>
+    <t>RSK</t>
+  </si>
+  <si>
+    <t>Duration (min)</t>
+  </si>
+  <si>
+    <t>Data Generated (GB)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Margin</t>
   </si>
 </sst>
 </file>
@@ -163,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -360,6 +383,47 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -371,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -416,7 +480,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -425,16 +499,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
@@ -533,6 +623,158 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Data Budget</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('For Pie'!$A$2:$A$4,'For Pie'!$B$5)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>ISK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Transition</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RSK</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Margin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('For Pie'!$C$2:$C$4,'For Pie'!$C$6)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.4312760000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4312760000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2156380000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9218099999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8632031" cy="6293304"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -824,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,14 +1078,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -853,9 +1095,9 @@
         <v>28</v>
       </c>
       <c r="C2" s="22">
-        <v>60</v>
-      </c>
-      <c r="D2" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="23"/>
@@ -868,7 +1110,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="23">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>31</v>
@@ -882,7 +1124,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="23">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>31</v>
@@ -931,7 +1173,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +1220,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -990,16 +1232,16 @@
       </c>
       <c r="D4" s="21">
         <f>fps/ISKS</f>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E4" s="18">
         <f>C4*(60*D4)</f>
-        <v>294900000</v>
+        <v>196600000</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1023,7 +1265,7 @@
       <c r="C6" s="13"/>
       <c r="E6" s="19">
         <f>SUM(E4:E5)</f>
-        <v>295245600</v>
+        <v>196945600</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -1047,7 +1289,7 @@
       <c r="C8" s="13"/>
       <c r="E8" s="19">
         <f>E7*E6</f>
-        <v>53144208000</v>
+        <v>35450208000</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -1095,7 +1337,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1107,16 +1349,16 @@
       </c>
       <c r="D13" s="21">
         <f>fps/TS</f>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E13" s="18">
         <f>C13*(60*D13)</f>
-        <v>294900000</v>
+        <v>196600000</v>
       </c>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
@@ -1140,7 +1382,7 @@
       <c r="C15" s="13"/>
       <c r="E15" s="19">
         <f>SUM(E13:E14)</f>
-        <v>295245600</v>
+        <v>196945600</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1164,7 +1406,7 @@
       <c r="C17" s="13"/>
       <c r="E17" s="19">
         <f>E16*E15</f>
-        <v>53144208000</v>
+        <v>35450208000</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -1206,7 +1448,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1218,16 +1460,16 @@
       </c>
       <c r="D22" s="21">
         <f>fps/RSKS</f>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E22" s="18">
         <f>C22*(60*D22)</f>
-        <v>294900000</v>
+        <v>196600000</v>
       </c>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
@@ -1251,7 +1493,7 @@
       <c r="C24" s="13"/>
       <c r="E24" s="19">
         <f>SUM(E22:E23)</f>
-        <v>295245600</v>
+        <v>196945600</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1275,7 +1517,7 @@
       <c r="C26" s="13"/>
       <c r="E26" s="19">
         <f>E25*E24</f>
-        <v>26572104000</v>
+        <v>17725104000</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1283,8 +1525,8 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E28" s="19">
-        <f>SUM(E8,E15,E26)</f>
-        <v>80011557600</v>
+        <f>SUM(E8,E17,E26)</f>
+        <v>88625520000</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
@@ -1302,7 +1544,7 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="20">
         <f>0.125*E28*(10^-9)</f>
-        <v>10.0014447</v>
+        <v>11.078190000000001</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
@@ -1315,49 +1557,141 @@
     <mergeCell ref="A22:A23"/>
   </mergeCells>
   <conditionalFormatting sqref="E7 C4:E5">
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16 D14:E14 C13:D13">
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25 D23:E23 C22:D22">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
       <formula>$E$29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
       <formula>$E$29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2" s="21">
+        <f>'Data Budget'!E8*0.125*(10^-9)</f>
+        <v>4.4312760000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7">
+        <v>180</v>
+      </c>
+      <c r="C3" s="21">
+        <f>'Data Budget'!E17*0.125*(10^-9)</f>
+        <v>4.4312760000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="29">
+        <v>90</v>
+      </c>
+      <c r="C4" s="28">
+        <f>'Data Budget'!E26*0.125*(10^-9)</f>
+        <v>2.2156380000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="30">
+        <f>(mem*0.25)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="21">
+        <f>mem-SUM(C2:C4)</f>
+        <v>4.9218099999999989</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="20"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
What did i do?
</commit_message>
<xml_diff>
--- a/RCL-B-CDH1 Data Budget.xlsx
+++ b/RCL-B-CDH1 Data Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="12600" windowHeight="12390" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="0" windowWidth="12600" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="2" r:id="rId1"/>
@@ -504,27 +504,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
@@ -690,16 +670,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.4312760000000004</c:v>
+                  <c:v>4.4338680000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4312760000000004</c:v>
+                  <c:v>4.4338680000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2156380000000002</c:v>
+                  <c:v>2.2169340000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9218099999999989</c:v>
+                  <c:v>4.9153299999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -743,7 +723,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -754,7 +734,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8632031" cy="6293304"/>
+    <xdr:ext cx="8643347" cy="6297521"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1067,7 +1047,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,8 +1226,8 @@
         <v>13</v>
       </c>
       <c r="C5" s="7">
-        <f>24*8</f>
-        <v>192</v>
+        <f>32*8</f>
+        <v>256</v>
       </c>
       <c r="D5" s="7">
         <f>fps</f>
@@ -1255,7 +1235,7 @@
       </c>
       <c r="E5" s="17">
         <f>C5*60*D5</f>
-        <v>345600</v>
+        <v>460800</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -1265,7 +1245,7 @@
       <c r="C6" s="13"/>
       <c r="E6" s="19">
         <f>SUM(E4:E5)</f>
-        <v>196945600</v>
+        <v>197060800</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -1289,7 +1269,7 @@
       <c r="C8" s="13"/>
       <c r="E8" s="19">
         <f>E7*E6</f>
-        <v>35450208000</v>
+        <v>35470944000</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -1363,8 +1343,8 @@
         <v>13</v>
       </c>
       <c r="C14" s="7">
-        <f>24*8</f>
-        <v>192</v>
+        <f>C5</f>
+        <v>256</v>
       </c>
       <c r="D14" s="7">
         <f>fps</f>
@@ -1372,7 +1352,7 @@
       </c>
       <c r="E14" s="17">
         <f>C14*60*D14</f>
-        <v>345600</v>
+        <v>460800</v>
       </c>
       <c r="F14" s="6"/>
     </row>
@@ -1382,7 +1362,7 @@
       <c r="C15" s="13"/>
       <c r="E15" s="19">
         <f>SUM(E13:E14)</f>
-        <v>196945600</v>
+        <v>197060800</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1406,7 +1386,7 @@
       <c r="C17" s="13"/>
       <c r="E17" s="19">
         <f>E16*E15</f>
-        <v>35450208000</v>
+        <v>35470944000</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -1474,8 +1454,8 @@
         <v>13</v>
       </c>
       <c r="C23" s="7">
-        <f>24*8</f>
-        <v>192</v>
+        <f>C5</f>
+        <v>256</v>
       </c>
       <c r="D23" s="7">
         <f>fps</f>
@@ -1483,7 +1463,7 @@
       </c>
       <c r="E23" s="17">
         <f>C23*60*D23</f>
-        <v>345600</v>
+        <v>460800</v>
       </c>
       <c r="F23" s="6"/>
     </row>
@@ -1493,7 +1473,7 @@
       <c r="C24" s="13"/>
       <c r="E24" s="19">
         <f>SUM(E22:E23)</f>
-        <v>196945600</v>
+        <v>197060800</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1517,7 +1497,7 @@
       <c r="C26" s="13"/>
       <c r="E26" s="19">
         <f>E25*E24</f>
-        <v>17725104000</v>
+        <v>17735472000</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1526,7 +1506,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E28" s="19">
         <f>SUM(E8,E17,E26)</f>
-        <v>88625520000</v>
+        <v>88677360000</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
@@ -1544,7 +1524,7 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="20">
         <f>0.125*E28*(10^-9)</f>
-        <v>11.078190000000001</v>
+        <v>11.084670000000001</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
@@ -1557,45 +1537,45 @@
     <mergeCell ref="A22:A23"/>
   </mergeCells>
   <conditionalFormatting sqref="E7 C4:E5">
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16 D14:E14 C13:D13">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25 D23:E23 C22:D22">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>$E$29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>$E$29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1639,7 +1619,7 @@
       </c>
       <c r="C2" s="21">
         <f>'Data Budget'!E8*0.125*(10^-9)</f>
-        <v>4.4312760000000004</v>
+        <v>4.4338680000000004</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1651,7 +1631,7 @@
       </c>
       <c r="C3" s="21">
         <f>'Data Budget'!E17*0.125*(10^-9)</f>
-        <v>4.4312760000000004</v>
+        <v>4.4338680000000004</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1663,7 +1643,7 @@
       </c>
       <c r="C4" s="28">
         <f>'Data Budget'!E26*0.125*(10^-9)</f>
-        <v>2.2156380000000002</v>
+        <v>2.2169340000000002</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1681,7 +1661,7 @@
       </c>
       <c r="C6" s="21">
         <f>mem-SUM(C2:C4)</f>
-        <v>4.9218099999999989</v>
+        <v>4.9153299999999991</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tweaked the data budget
</commit_message>
<xml_diff>
--- a/RCL-B-CDH1 Data Budget.xlsx
+++ b/RCL-B-CDH1 Data Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="12600" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="0" windowWidth="12600" windowHeight="12390" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="2" r:id="rId1"/>
@@ -504,7 +504,47 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
@@ -670,16 +710,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.4338680000000004</c:v>
+                  <c:v>4.6041895384615392</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4338680000000004</c:v>
+                  <c:v>4.6041895384615392</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2169340000000002</c:v>
+                  <c:v>2.3020947692307696</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9153299999999991</c:v>
+                  <c:v>4.4895261538461515</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,7 +763,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1047,7 +1087,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1115,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="22">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>31</v>
@@ -1090,7 +1130,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="23">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>31</v>
@@ -1104,7 +1144,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="23">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>31</v>
@@ -1152,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,16 +1247,16 @@
         <v>11</v>
       </c>
       <c r="C4" s="7">
-        <f>9.83*10^6</f>
-        <v>9830000</v>
+        <f>640*480*24</f>
+        <v>7372800</v>
       </c>
       <c r="D4" s="21">
         <f>fps/ISKS</f>
-        <v>0.33333333333333331</v>
+        <v>0.46153846153846156</v>
       </c>
       <c r="E4" s="18">
         <f>C4*(60*D4)</f>
-        <v>196600000</v>
+        <v>204169846.15384617</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -1245,7 +1285,7 @@
       <c r="C6" s="13"/>
       <c r="E6" s="19">
         <f>SUM(E4:E5)</f>
-        <v>197060800</v>
+        <v>204630646.15384617</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -1269,7 +1309,7 @@
       <c r="C8" s="13"/>
       <c r="E8" s="19">
         <f>E7*E6</f>
-        <v>35470944000</v>
+        <v>36833516307.692314</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -1324,16 +1364,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="7">
-        <f>9.83*10^6</f>
-        <v>9830000</v>
+        <f>640*480*24</f>
+        <v>7372800</v>
       </c>
       <c r="D13" s="21">
         <f>fps/TS</f>
-        <v>0.33333333333333331</v>
+        <v>0.46153846153846156</v>
       </c>
       <c r="E13" s="18">
         <f>C13*(60*D13)</f>
-        <v>196600000</v>
+        <v>204169846.15384617</v>
       </c>
       <c r="F13" s="6"/>
     </row>
@@ -1362,7 +1402,7 @@
       <c r="C15" s="13"/>
       <c r="E15" s="19">
         <f>SUM(E13:E14)</f>
-        <v>197060800</v>
+        <v>204630646.15384617</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -1386,7 +1426,7 @@
       <c r="C17" s="13"/>
       <c r="E17" s="19">
         <f>E16*E15</f>
-        <v>35470944000</v>
+        <v>36833516307.692314</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -1435,16 +1475,16 @@
         <v>11</v>
       </c>
       <c r="C22" s="7">
-        <f>9.83*10^6</f>
-        <v>9830000</v>
+        <f>640*480*24</f>
+        <v>7372800</v>
       </c>
       <c r="D22" s="21">
         <f>fps/RSKS</f>
-        <v>0.33333333333333331</v>
+        <v>0.46153846153846156</v>
       </c>
       <c r="E22" s="18">
         <f>C22*(60*D22)</f>
-        <v>196600000</v>
+        <v>204169846.15384617</v>
       </c>
       <c r="F22" s="6"/>
     </row>
@@ -1473,7 +1513,7 @@
       <c r="C24" s="13"/>
       <c r="E24" s="19">
         <f>SUM(E22:E23)</f>
-        <v>197060800</v>
+        <v>204630646.15384617</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -1497,7 +1537,7 @@
       <c r="C26" s="13"/>
       <c r="E26" s="19">
         <f>E25*E24</f>
-        <v>17735472000</v>
+        <v>18416758153.846157</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1506,7 +1546,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E28" s="19">
         <f>SUM(E8,E17,E26)</f>
-        <v>88677360000</v>
+        <v>92083790769.230789</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
@@ -1524,7 +1564,7 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="20">
         <f>0.125*E28*(10^-9)</f>
-        <v>11.084670000000001</v>
+        <v>11.510473846153848</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
@@ -1537,45 +1577,55 @@
     <mergeCell ref="A22:A23"/>
   </mergeCells>
   <conditionalFormatting sqref="E7 C4:E5">
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16 D14:E14 C13:D13">
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+  <conditionalFormatting sqref="E16 D14:E14 D13">
+    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25 D23:E23 C22:D22">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+  <conditionalFormatting sqref="E25 D23:E23 D22">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>$E$29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>$E$29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1619,7 +1669,7 @@
       </c>
       <c r="C2" s="21">
         <f>'Data Budget'!E8*0.125*(10^-9)</f>
-        <v>4.4338680000000004</v>
+        <v>4.6041895384615392</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1631,7 +1681,7 @@
       </c>
       <c r="C3" s="21">
         <f>'Data Budget'!E17*0.125*(10^-9)</f>
-        <v>4.4338680000000004</v>
+        <v>4.6041895384615392</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1643,7 +1693,7 @@
       </c>
       <c r="C4" s="28">
         <f>'Data Budget'!E26*0.125*(10^-9)</f>
-        <v>2.2169340000000002</v>
+        <v>2.3020947692307696</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1661,7 +1711,7 @@
       </c>
       <c r="C6" s="21">
         <f>mem-SUM(C2:C4)</f>
-        <v>4.9153299999999991</v>
+        <v>4.4895261538461515</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>